<commit_message>
Minor changes + added file - Added DomainModel.png - Changed User Story Wireframe
</commit_message>
<xml_diff>
--- a/analysis/Wireframe.xlsx
+++ b/analysis/Wireframe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szypk\Documents\GitHub\UCLL\FsSd\project2425-group3-17\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF8A885-6AC3-4082-B6A2-AA492797651A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AD2B45-9940-402A-9E55-987821D8BE25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>User</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>isSolved</t>
+  </si>
+  <si>
+    <t>details</t>
+  </si>
+  <si>
+    <t>aboutMe</t>
+  </si>
+  <si>
+    <t>textIncluded</t>
   </si>
 </sst>
 </file>
@@ -430,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -441,7 +450,8 @@
     <col min="3" max="3" width="18.109375" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" customWidth="1"/>
     <col min="5" max="5" width="21.33203125" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.3">
@@ -460,7 +470,9 @@
       <c r="E1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -502,7 +514,9 @@
       <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -554,7 +568,9 @@
       <c r="E6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -575,7 +591,9 @@
       <c r="E7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>

</xml_diff>